<commit_message>
Expence category testcases added
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTestData/testData.xlsx
+++ b/src/test/resources/ExcelTestData/testData.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="testData_Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="testcases" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Username</t>
   </si>
@@ -25,6 +25,12 @@
   </si>
   <si>
     <t>admin</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Testcase</t>
   </si>
 </sst>
 </file>
@@ -390,12 +396,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A3:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>